<commit_message>
NM Transp file updates and elec fixes
</commit_message>
<xml_diff>
--- a/InputData/indst/BNRbI/BAU Nonfuel Revenue by Industry.xlsx
+++ b/InputData/indst/BNRbI/BAU Nonfuel Revenue by Industry.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-virginia\InputData\indst\TNRbI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\RMI\New Mexico\NM_model\InputData\indst\BNRbI\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{083518AA-5D1C-4231-9CA2-A1DA79AA2E5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2978" yWindow="1103" windowWidth="24758" windowHeight="15578"/>
+    <workbookView xWindow="1215" yWindow="630" windowWidth="13170" windowHeight="16650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,18 @@
   <definedNames>
     <definedName name="currency_conv">About!$A$65</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -561,7 +573,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -808,15 +820,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Body: normal cell" xfId="5"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="7"/>
-    <cellStyle name="Footnotes: top row" xfId="3"/>
-    <cellStyle name="Header: bottom row" xfId="6"/>
+    <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Header: bottom row" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Parent row" xfId="4"/>
-    <cellStyle name="Table title" xfId="8"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Parent row" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Table title" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1151,23 +1163,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1175,267 +1187,267 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="27" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" s="27" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>2019</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B24" s="27" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>2019</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="24">
         <f>1.07*10^9</f>
         <v>1070000000.0000001</v>
@@ -1444,7 +1456,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>0.93665959530026111</v>
       </c>
@@ -1452,7 +1464,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>0.9143273584567535</v>
       </c>
@@ -1462,16 +1474,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B14" r:id="rId1"/>
-    <hyperlink ref="B21" r:id="rId2"/>
-    <hyperlink ref="B28" r:id="rId3"/>
+    <hyperlink ref="B14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B21" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B28" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1481,15 +1493,15 @@
       <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.796875" style="21" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="45.6640625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="9.1328125" style="21" customWidth="1"/>
-    <col min="4" max="16384" width="9.1328125" style="21"/>
+    <col min="1" max="1" width="20.85546875" style="21" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" style="21" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="21" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="13" t="s">
         <v>54</v>
       </c>
@@ -1596,8 +1608,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="15" t="s">
         <v>55</v>
       </c>
@@ -1608,7 +1620,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="15" t="s">
         <v>56</v>
       </c>
@@ -1621,7 +1633,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="15" t="s">
         <v>59</v>
       </c>
@@ -1632,7 +1644,7 @@
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="15" t="s">
         <v>61</v>
       </c>
@@ -1643,7 +1655,7 @@
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="10" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>63</v>
       </c>
@@ -1651,10 +1663,10 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="13"/>
     </row>
-    <row r="12" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="13"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
@@ -1694,7 +1706,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
         <v>66</v>
       </c>
@@ -1804,8 +1816,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="14" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>67</v>
       </c>
@@ -1918,7 +1930,7 @@
         <v>1.8898000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>69</v>
       </c>
@@ -2031,17 +2043,17 @@
         <v>5.8120000000000003E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>73</v>
       </c>
@@ -2154,7 +2166,7 @@
         <v>1.1761000000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>75</v>
       </c>
@@ -2267,7 +2279,7 @@
         <v>1.107E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>77</v>
       </c>
@@ -2380,12 +2392,12 @@
         <v>1.4662E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>80</v>
       </c>
@@ -2498,7 +2510,7 @@
         <v>1.7756000000000001E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>82</v>
       </c>
@@ -2611,7 +2623,7 @@
         <v>6.1960000000000001E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>84</v>
       </c>
@@ -2724,7 +2736,7 @@
         <v>-1.7729999999999999E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>86</v>
       </c>
@@ -2837,7 +2849,7 @@
         <v>1.0227999999999999E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>88</v>
       </c>
@@ -2950,7 +2962,7 @@
         <v>1.4657999999999999E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>90</v>
       </c>
@@ -3063,7 +3075,7 @@
         <v>9.9909999999999999E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
         <v>92</v>
       </c>
@@ -3176,7 +3188,7 @@
         <v>1.7110000000000001E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
         <v>94</v>
       </c>
@@ -3289,7 +3301,7 @@
         <v>1.9053E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>96</v>
       </c>
@@ -3402,7 +3414,7 @@
         <v>1.5769999999999999E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
         <v>98</v>
       </c>
@@ -3515,7 +3527,7 @@
         <v>-2.7539999999999999E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>100</v>
       </c>
@@ -3628,7 +3640,7 @@
         <v>1.9487000000000001E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
         <v>102</v>
       </c>
@@ -3741,7 +3753,7 @@
         <v>1.8273000000000001E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
         <v>104</v>
       </c>
@@ -3854,7 +3866,7 @@
         <v>5.829E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
         <v>106</v>
       </c>
@@ -3967,7 +3979,7 @@
         <v>2.2030000000000001E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
         <v>108</v>
       </c>
@@ -4080,7 +4092,7 @@
         <v>-2.575E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
         <v>110</v>
       </c>
@@ -4193,7 +4205,7 @@
         <v>-2.4510000000000001E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
         <v>112</v>
       </c>
@@ -4306,7 +4318,7 @@
         <v>-4.176E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
         <v>114</v>
       </c>
@@ -4419,7 +4431,7 @@
         <v>2.3494999999999999E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
         <v>116</v>
       </c>
@@ -4532,7 +4544,7 @@
         <v>1.8002000000000001E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
         <v>118</v>
       </c>
@@ -4645,7 +4657,7 @@
         <v>1.2220999999999999E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
         <v>120</v>
       </c>
@@ -4758,7 +4770,7 @@
         <v>1.6796999999999999E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
         <v>122</v>
       </c>
@@ -4871,7 +4883,7 @@
         <v>1.9954E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
         <v>124</v>
       </c>
@@ -4984,7 +4996,7 @@
         <v>9.5680000000000001E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
         <v>126</v>
       </c>
@@ -5097,7 +5109,7 @@
         <v>-7.7800000000000005E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
         <v>128</v>
       </c>
@@ -5210,7 +5222,7 @@
         <v>8.8459999999999997E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
         <v>130</v>
       </c>
@@ -5323,7 +5335,7 @@
         <v>2.0156E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
         <v>132</v>
       </c>
@@ -5436,7 +5448,7 @@
         <v>1.8870000000000001E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
         <v>134</v>
       </c>
@@ -5549,7 +5561,7 @@
         <v>2.6143E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
         <v>136</v>
       </c>
@@ -5662,7 +5674,7 @@
         <v>2.5361000000000002E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
         <v>138</v>
       </c>
@@ -5775,7 +5787,7 @@
         <v>2.5756000000000001E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
         <v>140</v>
       </c>
@@ -5888,7 +5900,7 @@
         <v>2.6575999999999999E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
         <v>142</v>
       </c>
@@ -6001,7 +6013,7 @@
         <v>2.8815E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="17" t="s">
         <v>144</v>
       </c>
@@ -6114,8 +6126,8 @@
         <v>1.7311E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="62" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="33" t="s">
         <v>146</v>
       </c>
@@ -6155,17 +6167,17 @@
       <c r="AJ62" s="34"/>
       <c r="AK62" s="34"/>
     </row>
-    <row r="63" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="64" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="65" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B65" s="4" t="s">
         <v>149</v>
       </c>
@@ -6180,35 +6192,35 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AJ22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="14.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.46484375" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>150</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>152</v>
       </c>
@@ -6229,7 +6241,7 @@
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2017</v>
       </c>
@@ -6243,17 +6255,17 @@
         <v>325084.75799999997</v>
       </c>
       <c r="E5">
-        <v>8466.7489999999998</v>
+        <v>2084.9540000000002</v>
       </c>
       <c r="F5">
         <f>B5*(E5/D5)</f>
-        <v>4.4796958090542036</v>
+        <v>1.1031341186411454</v>
       </c>
       <c r="G5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B6" s="31">
         <f>B5/About!A67</f>
         <v>183.63127956305479</v>
@@ -6263,25 +6275,25 @@
       </c>
       <c r="F6">
         <f>F5/About!A67</f>
-        <v>4.7826294969178917</v>
+        <v>1.1777321496263733</v>
       </c>
       <c r="G6" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
         <v>160</v>
       </c>
       <c r="B8" s="30"/>
       <c r="C8" s="30"/>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>152</v>
       </c>
@@ -6296,7 +6308,7 @@
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>2018</v>
       </c>
@@ -6308,13 +6320,13 @@
       </c>
       <c r="F12">
         <f>B12*(E5/D5)</f>
-        <v>1.8752215014645506</v>
+        <v>0.46177707291954923</v>
       </c>
       <c r="G12" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B13" s="31">
         <f>B12/About!A68</f>
         <v>78.746413233795309</v>
@@ -6324,20 +6336,20 @@
       </c>
       <c r="F13">
         <f>F12/About!A67</f>
-        <v>2.0020309521981874</v>
+        <v>0.49300415565755162</v>
       </c>
       <c r="G13" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>163</v>
       </c>
       <c r="B15" s="30"/>
       <c r="C15" s="30"/>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>152</v>
       </c>
@@ -6447,7 +6459,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>164</v>
       </c>
@@ -6455,528 +6467,528 @@
         <v>323015.99200000003</v>
       </c>
       <c r="C17" s="28">
-        <v>8466.7489999999998</v>
+        <v>2084.9540000000002</v>
       </c>
       <c r="D17" s="28">
-        <v>8533.2810000000009</v>
+        <v>2088.6370000000002</v>
       </c>
       <c r="E17" s="28">
-        <v>8599.8130000000001</v>
+        <v>2092.319</v>
       </c>
       <c r="F17" s="28">
-        <v>8666.3449999999993</v>
+        <v>2096.0010000000002</v>
       </c>
       <c r="G17" s="28">
-        <v>8732.8770000000004</v>
+        <v>2099.683</v>
       </c>
       <c r="H17" s="28">
-        <v>8799.4089999999997</v>
+        <v>2103.3649999999998</v>
       </c>
       <c r="I17" s="28">
-        <v>8865.9410000000007</v>
+        <v>2107.0479999999998</v>
       </c>
       <c r="J17" s="28">
-        <v>8932.473</v>
+        <v>2110.73</v>
       </c>
       <c r="K17" s="28">
-        <v>8999.0059999999994</v>
+        <v>2114.4119999999998</v>
       </c>
       <c r="L17" s="28">
-        <v>9065.5380000000005</v>
+        <v>2118.0940000000001</v>
       </c>
       <c r="M17" s="28">
-        <v>9132.07</v>
+        <v>2121.7759999999998</v>
       </c>
       <c r="N17" s="28">
-        <v>9198.6020000000008</v>
+        <v>2125.4589999999998</v>
       </c>
       <c r="O17" s="28">
-        <v>9265.134</v>
+        <v>2129.1410000000001</v>
       </c>
       <c r="P17" s="28">
-        <v>9331.6660000000011</v>
+        <v>2132.8229999999999</v>
       </c>
       <c r="Q17" s="28">
-        <v>9398.1980000000003</v>
+        <v>2136.5050000000001</v>
       </c>
       <c r="R17" s="28">
-        <v>9464.73</v>
+        <v>2140.1869999999999</v>
       </c>
       <c r="S17" s="28">
-        <v>9531.2620000000006</v>
+        <v>2143.87</v>
       </c>
       <c r="T17" s="28">
-        <v>9597.7939999999999</v>
+        <v>2147.5520000000001</v>
       </c>
       <c r="U17" s="28">
-        <v>9664.3260000000009</v>
+        <v>2151.2339999999999</v>
       </c>
       <c r="V17" s="28">
-        <v>9730.8590000000004</v>
+        <v>2154.9160000000002</v>
       </c>
       <c r="W17" s="28">
-        <v>9797.3909999999996</v>
+        <v>2158.598</v>
       </c>
       <c r="X17" s="28">
-        <v>9863.9230000000007</v>
+        <v>2162.2809999999999</v>
       </c>
       <c r="Y17" s="28">
-        <v>9930.4549999999999</v>
+        <v>2165.9630000000002</v>
       </c>
       <c r="Z17" s="28">
-        <v>9996.987000000001</v>
+        <v>2169.645</v>
       </c>
       <c r="AA17" s="28">
-        <v>10063.519</v>
+        <v>2173.3270000000002</v>
       </c>
       <c r="AB17" s="28">
-        <v>10130.050999999999</v>
+        <v>2177.009</v>
       </c>
       <c r="AC17" s="28">
-        <v>10196.583000000001</v>
+        <v>2180.692</v>
       </c>
       <c r="AD17" s="28">
-        <v>10263.115</v>
+        <v>2184.3739999999998</v>
       </c>
       <c r="AE17" s="28">
-        <v>10329.647999999999</v>
+        <v>2188.056</v>
       </c>
       <c r="AF17" s="28">
-        <v>10396.18</v>
+        <v>2191.7379999999998</v>
       </c>
       <c r="AG17" s="28">
-        <v>10462.712</v>
+        <v>2195.42</v>
       </c>
       <c r="AH17" s="28">
-        <v>10529.244000000001</v>
+        <v>2199.1030000000001</v>
       </c>
       <c r="AI17" s="28">
-        <v>10595.776</v>
+        <v>2202.7849999999999</v>
       </c>
       <c r="AJ17" s="28">
-        <v>10662.308000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.45">
+        <v>2206.4670000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>165</v>
       </c>
       <c r="B19" s="30"/>
       <c r="C19" s="30"/>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>150</v>
       </c>
       <c r="C20" s="32">
         <f>F6</f>
-        <v>4.7826294969178917</v>
+        <v>1.1777321496263733</v>
       </c>
       <c r="D20" s="29">
         <f t="shared" ref="D20:AJ20" si="0">$C20*(D17/$C17)</f>
-        <v>4.8202115612602912</v>
+        <v>1.1798125732266418</v>
       </c>
       <c r="E20" s="29">
         <f t="shared" si="0"/>
-        <v>4.8577936256026906</v>
+        <v>1.1818924319549033</v>
       </c>
       <c r="F20" s="29">
         <f t="shared" si="0"/>
-        <v>4.8953756899450882</v>
+        <v>1.1839722906831651</v>
       </c>
       <c r="G20" s="29">
         <f t="shared" si="0"/>
-        <v>4.9329577542874876</v>
+        <v>1.1860521494114269</v>
       </c>
       <c r="H20" s="29">
         <f t="shared" si="0"/>
-        <v>4.9705398186298853</v>
+        <v>1.1881320081396884</v>
       </c>
       <c r="I20" s="29">
         <f t="shared" si="0"/>
-        <v>5.0081218829722856</v>
+        <v>1.1902124317399569</v>
       </c>
       <c r="J20" s="29">
         <f t="shared" si="0"/>
-        <v>5.0457039473146841</v>
+        <v>1.1922922904682187</v>
       </c>
       <c r="K20" s="29">
         <f t="shared" si="0"/>
-        <v>5.0832865765290887</v>
+        <v>1.1943721491964805</v>
       </c>
       <c r="L20" s="29">
         <f t="shared" si="0"/>
-        <v>5.120868640871489</v>
+        <v>1.1964520079247425</v>
       </c>
       <c r="M20" s="29">
         <f t="shared" si="0"/>
-        <v>5.1584507052138866</v>
+        <v>1.198531866653004</v>
       </c>
       <c r="N20" s="29">
         <f t="shared" si="0"/>
-        <v>5.196032769556286</v>
+        <v>1.2006122902532725</v>
       </c>
       <c r="O20" s="29">
         <f t="shared" si="0"/>
-        <v>5.2336148338986845</v>
+        <v>1.2026921489815343</v>
       </c>
       <c r="P20" s="29">
         <f t="shared" si="0"/>
-        <v>5.2711968982410848</v>
+        <v>1.2047720077097961</v>
       </c>
       <c r="Q20" s="29">
         <f t="shared" si="0"/>
-        <v>5.3087789625834825</v>
+        <v>1.2068518664380579</v>
       </c>
       <c r="R20" s="29">
         <f t="shared" si="0"/>
-        <v>5.346361026925881</v>
+        <v>1.2089317251663194</v>
       </c>
       <c r="S20" s="29">
         <f t="shared" si="0"/>
-        <v>5.3839430912682804</v>
+        <v>1.2110121487665879</v>
       </c>
       <c r="T20" s="29">
         <f t="shared" si="0"/>
-        <v>5.4215251556106789</v>
+        <v>1.2130920074948497</v>
       </c>
       <c r="U20" s="29">
         <f t="shared" si="0"/>
-        <v>5.4591072199530783</v>
+        <v>1.2151718662231115</v>
       </c>
       <c r="V20" s="29">
         <f t="shared" si="0"/>
-        <v>5.4966898491674838</v>
+        <v>1.2172517249513735</v>
       </c>
       <c r="W20" s="29">
         <f t="shared" si="0"/>
-        <v>5.5342719135098823</v>
+        <v>1.219331583679635</v>
       </c>
       <c r="X20" s="29">
         <f t="shared" si="0"/>
-        <v>5.5718539778522809</v>
+        <v>1.2214120072799035</v>
       </c>
       <c r="Y20" s="29">
         <f t="shared" si="0"/>
-        <v>5.6094360421946794</v>
+        <v>1.2234918660081655</v>
       </c>
       <c r="Z20" s="29">
         <f t="shared" si="0"/>
-        <v>5.6470181065370797</v>
+        <v>1.2255717247364271</v>
       </c>
       <c r="AA20" s="29">
         <f t="shared" si="0"/>
-        <v>5.6846001708794782</v>
+        <v>1.2276515834646888</v>
       </c>
       <c r="AB20" s="29">
         <f t="shared" si="0"/>
-        <v>5.7221822352218759</v>
+        <v>1.2297314421929504</v>
       </c>
       <c r="AC20" s="29">
         <f t="shared" si="0"/>
-        <v>5.7597642995642753</v>
+        <v>1.2318118657932189</v>
       </c>
       <c r="AD20" s="29">
         <f t="shared" si="0"/>
-        <v>5.7973463639066747</v>
+        <v>1.2338917245214807</v>
       </c>
       <c r="AE20" s="29">
         <f t="shared" si="0"/>
-        <v>5.8349289931210784</v>
+        <v>1.2359715832497424</v>
       </c>
       <c r="AF20" s="29">
         <f t="shared" si="0"/>
-        <v>5.8725110574634787</v>
+        <v>1.2380514419780042</v>
       </c>
       <c r="AG20" s="29">
         <f t="shared" si="0"/>
-        <v>5.9100931218058772</v>
+        <v>1.2401313007062662</v>
       </c>
       <c r="AH20" s="29">
         <f t="shared" si="0"/>
-        <v>5.9476751861482766</v>
+        <v>1.2422117243065343</v>
       </c>
       <c r="AI20" s="29">
         <f t="shared" si="0"/>
-        <v>5.9852572504906743</v>
+        <v>1.2442915830347963</v>
       </c>
       <c r="AJ20" s="29">
         <f t="shared" si="0"/>
-        <v>6.0228393148330746</v>
-      </c>
-    </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.45">
+        <v>1.246371441763058</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>166</v>
       </c>
       <c r="D21" s="32">
         <f>F13</f>
-        <v>2.0020309521981874</v>
+        <v>0.49300415565755162</v>
       </c>
       <c r="E21" s="29">
         <f t="shared" ref="E21:AJ21" si="1">$D21*(E17/$D17)</f>
-        <v>2.0176403201905986</v>
+        <v>0.49387325895368733</v>
       </c>
       <c r="F21" s="29">
         <f t="shared" si="1"/>
-        <v>2.0332496881830093</v>
+        <v>0.49474236224982315</v>
       </c>
       <c r="G21" s="29">
         <f t="shared" si="1"/>
-        <v>2.048859056175421</v>
+        <v>0.49561146554595886</v>
       </c>
       <c r="H21" s="29">
         <f t="shared" si="1"/>
-        <v>2.0644684241678313</v>
+        <v>0.49648056884209452</v>
       </c>
       <c r="I21" s="29">
         <f t="shared" si="1"/>
-        <v>2.0800777921602429</v>
+        <v>0.49734990817932107</v>
       </c>
       <c r="J21" s="29">
         <f t="shared" si="1"/>
-        <v>2.0956871601526537</v>
+        <v>0.49821901147545689</v>
       </c>
       <c r="K21" s="29">
         <f t="shared" si="1"/>
-        <v>2.1112967627595056</v>
+        <v>0.49908811477159259</v>
       </c>
       <c r="L21" s="29">
         <f t="shared" si="1"/>
-        <v>2.1269061307519173</v>
+        <v>0.49995721806772842</v>
       </c>
       <c r="M21" s="29">
         <f t="shared" si="1"/>
-        <v>2.142515498744328</v>
+        <v>0.50082632136386407</v>
       </c>
       <c r="N21" s="29">
         <f t="shared" si="1"/>
-        <v>2.1581248667367396</v>
+        <v>0.50169566070109062</v>
       </c>
       <c r="O21" s="29">
         <f t="shared" si="1"/>
-        <v>2.1737342347291504</v>
+        <v>0.50256476399722638</v>
       </c>
       <c r="P21" s="29">
         <f t="shared" si="1"/>
-        <v>2.1893436027215616</v>
+        <v>0.50343386729336215</v>
       </c>
       <c r="Q21" s="29">
         <f t="shared" si="1"/>
-        <v>2.2049529707139723</v>
+        <v>0.50430297058949791</v>
       </c>
       <c r="R21" s="29">
         <f t="shared" si="1"/>
-        <v>2.2205623387063835</v>
+        <v>0.50517207388563368</v>
       </c>
       <c r="S21" s="29">
         <f t="shared" si="1"/>
-        <v>2.2361717066987947</v>
+        <v>0.50604141322286023</v>
       </c>
       <c r="T21" s="29">
         <f t="shared" si="1"/>
-        <v>2.2517810746912059</v>
+        <v>0.50691051651899599</v>
       </c>
       <c r="U21" s="29">
         <f t="shared" si="1"/>
-        <v>2.2673904426836171</v>
+        <v>0.50777961981513164</v>
       </c>
       <c r="V21" s="29">
         <f t="shared" si="1"/>
-        <v>2.2830000452904691</v>
+        <v>0.50864872311126752</v>
       </c>
       <c r="W21" s="29">
         <f t="shared" si="1"/>
-        <v>2.2986094132828803</v>
+        <v>0.50951782640740317</v>
       </c>
       <c r="X21" s="29">
         <f t="shared" si="1"/>
-        <v>2.3142187812752915</v>
+        <v>0.51038716574462972</v>
       </c>
       <c r="Y21" s="29">
         <f t="shared" si="1"/>
-        <v>2.3298281492677022</v>
+        <v>0.5112562690407656</v>
       </c>
       <c r="Z21" s="29">
         <f t="shared" si="1"/>
-        <v>2.3454375172601138</v>
+        <v>0.51212537233690125</v>
       </c>
       <c r="AA21" s="29">
         <f t="shared" si="1"/>
-        <v>2.3610468852525246</v>
+        <v>0.51299447563303702</v>
       </c>
       <c r="AB21" s="29">
         <f t="shared" si="1"/>
-        <v>2.3766562532449358</v>
+        <v>0.51386357892917278</v>
       </c>
       <c r="AC21" s="29">
         <f t="shared" si="1"/>
-        <v>2.392265621237347</v>
+        <v>0.51473291826639933</v>
       </c>
       <c r="AD21" s="29">
         <f t="shared" si="1"/>
-        <v>2.4078749892297582</v>
+        <v>0.51560202156253498</v>
       </c>
       <c r="AE21" s="29">
         <f t="shared" si="1"/>
-        <v>2.4234845918366101</v>
+        <v>0.51647112485867075</v>
       </c>
       <c r="AF21" s="29">
         <f t="shared" si="1"/>
-        <v>2.4390939598290213</v>
+        <v>0.51734022815480651</v>
       </c>
       <c r="AG21" s="29">
         <f t="shared" si="1"/>
-        <v>2.4547033278214321</v>
+        <v>0.51820933145094239</v>
       </c>
       <c r="AH21" s="29">
         <f t="shared" si="1"/>
-        <v>2.4703126958138433</v>
+        <v>0.51907867078816883</v>
       </c>
       <c r="AI21" s="29">
         <f t="shared" si="1"/>
-        <v>2.4859220638062545</v>
+        <v>0.51994777408430459</v>
       </c>
       <c r="AJ21" s="29">
         <f t="shared" si="1"/>
-        <v>2.5015314317986657</v>
-      </c>
-    </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.45">
+        <v>0.52081687738044036</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>167</v>
       </c>
       <c r="D22" s="29">
         <f t="shared" ref="D22:AJ22" si="2">SUM(D20:D21)</f>
-        <v>6.8222425134584785</v>
+        <v>1.6728167288841935</v>
       </c>
       <c r="E22" s="29">
         <f t="shared" si="2"/>
-        <v>6.8754339457932891</v>
+        <v>1.6757656909085907</v>
       </c>
       <c r="F22" s="29">
         <f t="shared" si="2"/>
-        <v>6.928625378128098</v>
+        <v>1.6787146529329884</v>
       </c>
       <c r="G22" s="29">
         <f t="shared" si="2"/>
-        <v>6.9818168104629086</v>
+        <v>1.6816636149573858</v>
       </c>
       <c r="H22" s="29">
         <f t="shared" si="2"/>
-        <v>7.0350082427977165</v>
+        <v>1.684612576981783</v>
       </c>
       <c r="I22" s="29">
         <f t="shared" si="2"/>
-        <v>7.0881996751325289</v>
+        <v>1.6875623399192781</v>
       </c>
       <c r="J22" s="29">
         <f t="shared" si="2"/>
-        <v>7.1413911074673377</v>
+        <v>1.6905113019436757</v>
       </c>
       <c r="K22" s="29">
         <f t="shared" si="2"/>
-        <v>7.1945833392885943</v>
+        <v>1.6934602639680731</v>
       </c>
       <c r="L22" s="29">
         <f t="shared" si="2"/>
-        <v>7.2477747716234067</v>
+        <v>1.696409225992471</v>
       </c>
       <c r="M22" s="29">
         <f t="shared" si="2"/>
-        <v>7.3009662039582146</v>
+        <v>1.699358188016868</v>
       </c>
       <c r="N22" s="29">
         <f t="shared" si="2"/>
-        <v>7.3541576362930261</v>
+        <v>1.702307950954363</v>
       </c>
       <c r="O22" s="29">
         <f t="shared" si="2"/>
-        <v>7.4073490686278349</v>
+        <v>1.7052569129787607</v>
       </c>
       <c r="P22" s="29">
         <f t="shared" si="2"/>
-        <v>7.4605405009626464</v>
+        <v>1.7082058750031583</v>
       </c>
       <c r="Q22" s="29">
         <f t="shared" si="2"/>
-        <v>7.5137319332974553</v>
+        <v>1.7111548370275558</v>
       </c>
       <c r="R22" s="29">
         <f t="shared" si="2"/>
-        <v>7.566923365632265</v>
+        <v>1.7141037990519532</v>
       </c>
       <c r="S22" s="29">
         <f t="shared" si="2"/>
-        <v>7.6201147979670747</v>
+        <v>1.7170535619894483</v>
       </c>
       <c r="T22" s="29">
         <f t="shared" si="2"/>
-        <v>7.6733062303018844</v>
+        <v>1.7200025240138457</v>
       </c>
       <c r="U22" s="29">
         <f t="shared" si="2"/>
-        <v>7.7264976626366959</v>
+        <v>1.7229514860382431</v>
       </c>
       <c r="V22" s="29">
         <f t="shared" si="2"/>
-        <v>7.7796898944579524</v>
+        <v>1.725900448062641</v>
       </c>
       <c r="W22" s="29">
         <f t="shared" si="2"/>
-        <v>7.8328813267927622</v>
+        <v>1.7288494100870382</v>
       </c>
       <c r="X22" s="29">
         <f t="shared" si="2"/>
-        <v>7.8860727591275719</v>
+        <v>1.7317991730245332</v>
       </c>
       <c r="Y22" s="29">
         <f t="shared" si="2"/>
-        <v>7.9392641914623816</v>
+        <v>1.7347481350489311</v>
       </c>
       <c r="Z22" s="29">
         <f t="shared" si="2"/>
-        <v>7.9924556237971931</v>
+        <v>1.7376970970733283</v>
       </c>
       <c r="AA22" s="29">
         <f t="shared" si="2"/>
-        <v>8.0456470561320028</v>
+        <v>1.7406460590977257</v>
       </c>
       <c r="AB22" s="29">
         <f t="shared" si="2"/>
-        <v>8.0988384884668108</v>
+        <v>1.7435950211221232</v>
       </c>
       <c r="AC22" s="29">
         <f t="shared" si="2"/>
-        <v>8.1520299208016223</v>
+        <v>1.7465447840596182</v>
       </c>
       <c r="AD22" s="29">
         <f t="shared" si="2"/>
-        <v>8.2052213531364337</v>
+        <v>1.7494937460840156</v>
       </c>
       <c r="AE22" s="29">
         <f t="shared" si="2"/>
-        <v>8.2584135849576885</v>
+        <v>1.7524427081084131</v>
       </c>
       <c r="AF22" s="29">
         <f t="shared" si="2"/>
-        <v>8.3116050172925</v>
+        <v>1.7553916701328107</v>
       </c>
       <c r="AG22" s="29">
         <f t="shared" si="2"/>
-        <v>8.3647964496273097</v>
+        <v>1.7583406321572086</v>
       </c>
       <c r="AH22" s="29">
         <f t="shared" si="2"/>
-        <v>8.4179878819621194</v>
+        <v>1.761290395094703</v>
       </c>
       <c r="AI22" s="29">
         <f t="shared" si="2"/>
-        <v>8.4711793142969292</v>
+        <v>1.7642393571191008</v>
       </c>
       <c r="AJ22" s="29">
         <f t="shared" si="2"/>
-        <v>8.5243707466317407</v>
+        <v>1.7671883191434983</v>
       </c>
     </row>
   </sheetData>
@@ -6986,23 +6998,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AH11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.46484375" customWidth="1"/>
-    <col min="2" max="2" width="11.46484375" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>168</v>
       </c>
@@ -7106,109 +7118,109 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>169</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24">
-        <v>297887963.88</v>
+        <v>115152406.68000001</v>
       </c>
       <c r="D2" s="24">
-        <v>294204135.42000002</v>
+        <v>113728375.62</v>
       </c>
       <c r="E2" s="24">
-        <v>296078513.12</v>
+        <v>114452940.31999999</v>
       </c>
       <c r="F2" s="24">
-        <v>302990449.06</v>
+        <v>117124837.66</v>
       </c>
       <c r="G2" s="24">
-        <v>309255107.98000002</v>
+        <v>119546521.78</v>
       </c>
       <c r="H2" s="24">
-        <v>314763463.56</v>
+        <v>121675847.16</v>
       </c>
       <c r="I2" s="24">
-        <v>320288723.56</v>
+        <v>123811707.16</v>
       </c>
       <c r="J2" s="24">
-        <v>324900200.04000002</v>
+        <v>125594332.44</v>
       </c>
       <c r="K2" s="24">
-        <v>329525273.99999988</v>
+        <v>127382214</v>
       </c>
       <c r="L2" s="24">
-        <v>334489073.10000002</v>
+        <v>129301034.09999999</v>
       </c>
       <c r="M2" s="24">
-        <v>339464744.31999987</v>
+        <v>131224443.52</v>
       </c>
       <c r="N2" s="24">
-        <v>344497455.11999989</v>
+        <v>133169902.31999999</v>
       </c>
       <c r="O2" s="24">
-        <v>349652440.54000002</v>
+        <v>135162627.94</v>
       </c>
       <c r="P2" s="24">
-        <v>354788878.33999997</v>
+        <v>137148183.74000001</v>
       </c>
       <c r="Q2" s="24">
-        <v>360030645.25999999</v>
+        <v>139174455.86000001</v>
       </c>
       <c r="R2" s="24">
-        <v>365926138.75999999</v>
+        <v>141453434.36000001</v>
       </c>
       <c r="S2" s="24">
-        <v>370911443.24000001</v>
+        <v>143380567.63999999</v>
       </c>
       <c r="T2" s="24">
-        <v>375417118.18000001</v>
+        <v>145122293.97999999</v>
       </c>
       <c r="U2" s="24">
-        <v>380053222.12</v>
+        <v>146914439.31999999</v>
       </c>
       <c r="V2" s="24">
-        <v>384205198.25999999</v>
+        <v>148519438.86000001</v>
       </c>
       <c r="W2" s="24">
-        <v>387463951.42000002</v>
+        <v>149779151.62</v>
       </c>
       <c r="X2" s="24">
-        <v>392775698.12</v>
+        <v>151832475.31999999</v>
       </c>
       <c r="Y2" s="24">
-        <v>398796300.75999999</v>
+        <v>154159816.36000001</v>
       </c>
       <c r="Z2" s="24">
-        <v>403602845.62</v>
+        <v>156017847.81999999</v>
       </c>
       <c r="AA2" s="24">
-        <v>409395433.72000003</v>
+        <v>158257046.91999999</v>
       </c>
       <c r="AB2" s="24">
-        <v>416123290.18000001</v>
+        <v>160857785.97999999</v>
       </c>
       <c r="AC2" s="24">
-        <v>423170974.98000002</v>
+        <v>163582158.78</v>
       </c>
       <c r="AD2" s="24">
-        <v>429837129.27999997</v>
+        <v>166159046.08000001</v>
       </c>
       <c r="AE2" s="24">
-        <v>436246204.94</v>
+        <v>168636556.34</v>
       </c>
       <c r="AF2" s="24">
-        <v>442783655.60000002</v>
+        <v>171163691.59999999</v>
       </c>
       <c r="AG2" s="24">
-        <v>449053470.06</v>
+        <v>173587368.66</v>
       </c>
       <c r="AH2" s="24">
-        <v>455356169.06</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
+        <v>176023757.66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>170</v>
       </c>
@@ -7309,211 +7321,211 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>171</v>
       </c>
       <c r="B4" s="24"/>
       <c r="C4" s="24">
-        <v>934978273.20000005</v>
+        <v>68379008.039999992</v>
       </c>
       <c r="D4" s="24">
-        <v>903072203.20000017</v>
+        <v>66045579.040000007</v>
       </c>
       <c r="E4" s="24">
-        <v>854109990.10000002</v>
+        <v>62464760.469999999</v>
       </c>
       <c r="F4" s="24">
-        <v>835140239.89999998</v>
+        <v>61077420.530000001</v>
       </c>
       <c r="G4" s="24">
-        <v>846017053.39999998</v>
+        <v>61872888.979999997</v>
       </c>
       <c r="H4" s="24">
-        <v>853630256.70000005</v>
+        <v>62429675.489999987</v>
       </c>
       <c r="I4" s="24">
-        <v>853253013.20000005</v>
+        <v>62402086.039999999</v>
       </c>
       <c r="J4" s="24">
-        <v>849876226.60000002</v>
+        <v>62155127.020000003</v>
       </c>
       <c r="K4" s="24">
-        <v>845194943.30000007</v>
+        <v>61812764.509999998</v>
       </c>
       <c r="L4" s="24">
-        <v>841080486.70000005</v>
+        <v>61511856.489999987</v>
       </c>
       <c r="M4" s="24">
-        <v>837520086.60000002</v>
+        <v>61251469.020000003</v>
       </c>
       <c r="N4" s="24">
-        <v>834125210</v>
+        <v>61003187</v>
       </c>
       <c r="O4" s="24">
-        <v>830309586.80000007</v>
+        <v>60724133.960000001</v>
       </c>
       <c r="P4" s="24">
-        <v>832031460</v>
+        <v>60850062</v>
       </c>
       <c r="Q4" s="24">
-        <v>834659890.10000002</v>
+        <v>61042290.469999999</v>
       </c>
       <c r="R4" s="24">
-        <v>836330186.70000005</v>
+        <v>61164446.489999987</v>
       </c>
       <c r="S4" s="24">
-        <v>838302639.89999998</v>
+        <v>61308700.530000001</v>
       </c>
       <c r="T4" s="24">
-        <v>840887520</v>
+        <v>61497744</v>
       </c>
       <c r="U4" s="24">
-        <v>844038523.30000007</v>
+        <v>61728190.509999998</v>
       </c>
       <c r="V4" s="24">
-        <v>846317213.39999998</v>
+        <v>61894840.979999997</v>
       </c>
       <c r="W4" s="24">
-        <v>847735603.39999998</v>
+        <v>61998573.979999997</v>
       </c>
       <c r="X4" s="24">
-        <v>849692666.70000005</v>
+        <v>62141702.489999987</v>
       </c>
       <c r="Y4" s="24">
-        <v>849255156.70000005</v>
+        <v>62109705.489999987</v>
       </c>
       <c r="Z4" s="24">
-        <v>848771389.89999998</v>
+        <v>62074325.530000001</v>
       </c>
       <c r="AA4" s="24">
-        <v>848112800</v>
+        <v>62026160</v>
       </c>
       <c r="AB4" s="24">
-        <v>846827049.89999998</v>
+        <v>61932127.530000001</v>
       </c>
       <c r="AC4" s="24">
-        <v>844971149.89999998</v>
+        <v>61796397.530000001</v>
       </c>
       <c r="AD4" s="24">
-        <v>843383256.60000002</v>
+        <v>61680268.020000003</v>
       </c>
       <c r="AE4" s="24">
-        <v>839159616.80000007</v>
+        <v>61371374.960000001</v>
       </c>
       <c r="AF4" s="24">
-        <v>836344243.30000007</v>
+        <v>61165474.509999998</v>
       </c>
       <c r="AG4" s="24">
-        <v>832796579.89999998</v>
+        <v>60906018.530000001</v>
       </c>
       <c r="AH4" s="24">
-        <v>827677109.89999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
+        <v>60531609.530000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>172</v>
       </c>
       <c r="B5" s="24"/>
       <c r="C5" s="24">
-        <v>7276429538.6399994</v>
+        <v>768946358.25</v>
       </c>
       <c r="D5" s="24">
-        <v>7424639203.6799994</v>
+        <v>784608611.5</v>
       </c>
       <c r="E5" s="24">
-        <v>7719965954.6399994</v>
+        <v>815817658.25</v>
       </c>
       <c r="F5" s="24">
-        <v>7971518962.079999</v>
+        <v>842400856.5</v>
       </c>
       <c r="G5" s="24">
-        <v>8230387713.8399992</v>
+        <v>869757155.75</v>
       </c>
       <c r="H5" s="24">
-        <v>8431239366.7199993</v>
+        <v>890982421</v>
       </c>
       <c r="I5" s="24">
-        <v>8585335101.6000004</v>
+        <v>907266692.50000012</v>
       </c>
       <c r="J5" s="24">
-        <v>8715539923.1999989</v>
+        <v>921026259.99999988</v>
       </c>
       <c r="K5" s="24">
-        <v>8840767852.0799999</v>
+        <v>934259887.75</v>
       </c>
       <c r="L5" s="24">
-        <v>8979370928.6399975</v>
+        <v>948906951.99999988</v>
       </c>
       <c r="M5" s="24">
-        <v>9114756811.1999989</v>
+        <v>963214035</v>
       </c>
       <c r="N5" s="24">
-        <v>9269476179.1199989</v>
+        <v>979564209.75</v>
       </c>
       <c r="O5" s="24">
-        <v>9400622999.7599983</v>
+        <v>993423324.25</v>
       </c>
       <c r="P5" s="24">
-        <v>9525147443.2799988</v>
+        <v>1006582610.25</v>
       </c>
       <c r="Q5" s="24">
-        <v>9651522566.1599998</v>
+        <v>1019937469.25</v>
       </c>
       <c r="R5" s="24">
-        <v>9783485066.1599998</v>
+        <v>1033882781.75</v>
       </c>
       <c r="S5" s="24">
-        <v>9921467556.7199993</v>
+        <v>1048464264.75</v>
       </c>
       <c r="T5" s="24">
-        <v>10041161663.52</v>
+        <v>1061113098.5</v>
       </c>
       <c r="U5" s="24">
-        <v>10159144592.4</v>
+        <v>1073581101.25</v>
       </c>
       <c r="V5" s="24">
-        <v>10279991954.16</v>
+        <v>1086351806.75</v>
       </c>
       <c r="W5" s="24">
-        <v>10408335994.799999</v>
+        <v>1099914733.75</v>
       </c>
       <c r="X5" s="24">
-        <v>10540618897.68</v>
+        <v>1113893905.25</v>
       </c>
       <c r="Y5" s="24">
-        <v>10664603617.68</v>
+        <v>1126996155.25</v>
       </c>
       <c r="Z5" s="24">
-        <v>10818140402.879999</v>
+        <v>1143221359</v>
       </c>
       <c r="AA5" s="24">
-        <v>10947445668.719999</v>
+        <v>1156885864.75</v>
       </c>
       <c r="AB5" s="24">
-        <v>11091089311.200001</v>
+        <v>1172065597.5</v>
       </c>
       <c r="AC5" s="24">
-        <v>11236097464.559999</v>
+        <v>1187389526.75</v>
       </c>
       <c r="AD5" s="24">
-        <v>11401615591.92</v>
+        <v>1204880874.75</v>
       </c>
       <c r="AE5" s="24">
-        <v>11544098908.32</v>
+        <v>1219937988.5</v>
       </c>
       <c r="AF5" s="24">
-        <v>11686892526</v>
+        <v>1235027893.75</v>
       </c>
       <c r="AG5" s="24">
-        <v>11855694551.040001</v>
+        <v>1252866272</v>
       </c>
       <c r="AH5" s="24">
-        <v>11976180076.799999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
+        <v>1265598740</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>173</v>
       </c>
@@ -7614,345 +7626,345 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>174</v>
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="24">
         <f>'water &amp; waste'!E22*10^9</f>
-        <v>6875433945.7932892</v>
+        <v>1675765690.9085908</v>
       </c>
       <c r="D7" s="24">
         <f>'water &amp; waste'!F22*10^9</f>
-        <v>6928625378.1280975</v>
+        <v>1678714652.9329884</v>
       </c>
       <c r="E7" s="24">
         <f>'water &amp; waste'!G22*10^9</f>
-        <v>6981816810.4629087</v>
+        <v>1681663614.9573858</v>
       </c>
       <c r="F7" s="24">
         <f>'water &amp; waste'!H22*10^9</f>
-        <v>7035008242.7977161</v>
+        <v>1684612576.9817829</v>
       </c>
       <c r="G7" s="24">
         <f>'water &amp; waste'!I22*10^9</f>
-        <v>7088199675.1325293</v>
+        <v>1687562339.9192781</v>
       </c>
       <c r="H7" s="24">
         <f>'water &amp; waste'!J22*10^9</f>
-        <v>7141391107.4673376</v>
+        <v>1690511301.9436758</v>
       </c>
       <c r="I7" s="24">
         <f>'water &amp; waste'!K22*10^9</f>
-        <v>7194583339.2885942</v>
+        <v>1693460263.9680731</v>
       </c>
       <c r="J7" s="24">
         <f>'water &amp; waste'!L22*10^9</f>
-        <v>7247774771.6234064</v>
+        <v>1696409225.992471</v>
       </c>
       <c r="K7" s="24">
         <f>'water &amp; waste'!M22*10^9</f>
-        <v>7300966203.9582148</v>
+        <v>1699358188.0168681</v>
       </c>
       <c r="L7" s="24">
         <f>'water &amp; waste'!N22*10^9</f>
-        <v>7354157636.293026</v>
+        <v>1702307950.9543631</v>
       </c>
       <c r="M7" s="24">
         <f>'water &amp; waste'!O22*10^9</f>
-        <v>7407349068.6278353</v>
+        <v>1705256912.9787607</v>
       </c>
       <c r="N7" s="24">
         <f>'water &amp; waste'!P22*10^9</f>
-        <v>7460540500.9626465</v>
+        <v>1708205875.0031583</v>
       </c>
       <c r="O7" s="24">
         <f>'water &amp; waste'!Q22*10^9</f>
-        <v>7513731933.2974548</v>
+        <v>1711154837.0275557</v>
       </c>
       <c r="P7" s="24">
         <f>'water &amp; waste'!R22*10^9</f>
-        <v>7566923365.6322651</v>
+        <v>1714103799.0519533</v>
       </c>
       <c r="Q7" s="24">
         <f>'water &amp; waste'!S22*10^9</f>
-        <v>7620114797.9670744</v>
+        <v>1717053561.9894483</v>
       </c>
       <c r="R7" s="24">
         <f>'water &amp; waste'!T22*10^9</f>
-        <v>7673306230.3018847</v>
+        <v>1720002524.0138457</v>
       </c>
       <c r="S7" s="24">
         <f>'water &amp; waste'!U22*10^9</f>
-        <v>7726497662.6366959</v>
+        <v>1722951486.0382431</v>
       </c>
       <c r="T7" s="24">
         <f>'water &amp; waste'!V22*10^9</f>
-        <v>7779689894.4579525</v>
+        <v>1725900448.0626409</v>
       </c>
       <c r="U7" s="24">
         <f>'water &amp; waste'!W22*10^9</f>
-        <v>7832881326.7927618</v>
+        <v>1728849410.0870383</v>
       </c>
       <c r="V7" s="24">
         <f>'water &amp; waste'!X22*10^9</f>
-        <v>7886072759.1275721</v>
+        <v>1731799173.0245333</v>
       </c>
       <c r="W7" s="24">
         <f>'water &amp; waste'!Y22*10^9</f>
-        <v>7939264191.4623814</v>
+        <v>1734748135.0489311</v>
       </c>
       <c r="X7" s="24">
         <f>'water &amp; waste'!Z22*10^9</f>
-        <v>7992455623.7971935</v>
+        <v>1737697097.0733283</v>
       </c>
       <c r="Y7" s="24">
         <f>'water &amp; waste'!AA22*10^9</f>
-        <v>8045647056.1320028</v>
+        <v>1740646059.0977256</v>
       </c>
       <c r="Z7" s="24">
         <f>'water &amp; waste'!AB22*10^9</f>
-        <v>8098838488.4668112</v>
+        <v>1743595021.1221232</v>
       </c>
       <c r="AA7" s="24">
         <f>'water &amp; waste'!AC22*10^9</f>
-        <v>8152029920.8016224</v>
+        <v>1746544784.0596182</v>
       </c>
       <c r="AB7" s="24">
         <f>'water &amp; waste'!AD22*10^9</f>
-        <v>8205221353.1364336</v>
+        <v>1749493746.0840156</v>
       </c>
       <c r="AC7" s="24">
         <f>'water &amp; waste'!AE22*10^9</f>
-        <v>8258413584.9576883</v>
+        <v>1752442708.108413</v>
       </c>
       <c r="AD7" s="24">
         <f>'water &amp; waste'!AF22*10^9</f>
-        <v>8311605017.2924995</v>
+        <v>1755391670.1328108</v>
       </c>
       <c r="AE7" s="24">
         <f>'water &amp; waste'!AG22*10^9</f>
-        <v>8364796449.6273098</v>
+        <v>1758340632.1572087</v>
       </c>
       <c r="AF7" s="24">
         <f>'water &amp; waste'!AH22*10^9</f>
-        <v>8417987881.9621191</v>
+        <v>1761290395.094703</v>
       </c>
       <c r="AG7" s="24">
         <f>'water &amp; waste'!AI22*10^9</f>
-        <v>8471179314.2969294</v>
+        <v>1764239357.1191008</v>
       </c>
       <c r="AH7" s="24">
         <f>'water &amp; waste'!AJ22*10^9</f>
-        <v>8524370746.6317406</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
+        <v>1767188319.1434982</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>175</v>
       </c>
       <c r="B8" s="24"/>
       <c r="C8" s="24">
-        <v>15081220277.76</v>
+        <v>1004724153.12</v>
       </c>
       <c r="D8" s="24">
-        <v>15265998267.52</v>
+        <v>1017034225.24</v>
       </c>
       <c r="E8" s="24">
-        <v>15531545848</v>
+        <v>1034725238.5</v>
       </c>
       <c r="F8" s="24">
-        <v>15820529524.799999</v>
+        <v>1053977585.1</v>
       </c>
       <c r="G8" s="24">
-        <v>16047274152</v>
+        <v>1069083511.5</v>
       </c>
       <c r="H8" s="24">
-        <v>16296562609.6</v>
+        <v>1085691327.7</v>
       </c>
       <c r="I8" s="24">
-        <v>16550104247.040001</v>
+        <v>1102582494.48</v>
       </c>
       <c r="J8" s="24">
-        <v>16788330511.68</v>
+        <v>1118453337.6600001</v>
       </c>
       <c r="K8" s="24">
-        <v>17023007426.879999</v>
+        <v>1134087720.0599999</v>
       </c>
       <c r="L8" s="24">
-        <v>17260935095.040001</v>
+        <v>1149938670.48</v>
       </c>
       <c r="M8" s="24">
-        <v>17505275424</v>
+        <v>1166216838</v>
       </c>
       <c r="N8" s="24">
-        <v>17764948918.080002</v>
+        <v>1183516514.46</v>
       </c>
       <c r="O8" s="24">
-        <v>18052384488.32</v>
+        <v>1202665724.8399999</v>
       </c>
       <c r="P8" s="24">
-        <v>18331662061.439999</v>
+        <v>1221271442.28</v>
       </c>
       <c r="Q8" s="24">
-        <v>18600499532.16</v>
+        <v>1239181630.9200001</v>
       </c>
       <c r="R8" s="24">
-        <v>18884846081.919998</v>
+        <v>1258125048.04</v>
       </c>
       <c r="S8" s="24">
-        <v>19155085884.48</v>
+        <v>1276128661.26</v>
       </c>
       <c r="T8" s="24">
-        <v>19406560467.84</v>
+        <v>1292882119.0799999</v>
       </c>
       <c r="U8" s="24">
-        <v>19646162390.400002</v>
+        <v>1308844609.8</v>
       </c>
       <c r="V8" s="24">
-        <v>19884040321.599998</v>
+        <v>1324692246.7</v>
       </c>
       <c r="W8" s="24">
-        <v>20118795424</v>
+        <v>1340331838</v>
       </c>
       <c r="X8" s="24">
-        <v>20368064342.080002</v>
+        <v>1356938352.46</v>
       </c>
       <c r="Y8" s="24">
-        <v>20622139166.720001</v>
+        <v>1373865040.6400001</v>
       </c>
       <c r="Z8" s="24">
-        <v>20871548501.439999</v>
+        <v>1390480909.78</v>
       </c>
       <c r="AA8" s="24">
-        <v>21131113552.639999</v>
+        <v>1407773361.6800001</v>
       </c>
       <c r="AB8" s="24">
-        <v>21397110833.279999</v>
+        <v>1425494334.3599999</v>
       </c>
       <c r="AC8" s="24">
-        <v>21670485840.639999</v>
+        <v>1443706817.6800001</v>
       </c>
       <c r="AD8" s="24">
-        <v>21945529773.439999</v>
+        <v>1462030486.28</v>
       </c>
       <c r="AE8" s="24">
-        <v>22221773450.240002</v>
+        <v>1480434082.8800001</v>
       </c>
       <c r="AF8" s="24">
-        <v>22500892843.52</v>
+        <v>1499029262.24</v>
       </c>
       <c r="AG8" s="24">
-        <v>22784121447.360001</v>
+        <v>1517898200.8199999</v>
       </c>
       <c r="AH8" s="24">
-        <v>23070453311.360001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
+        <v>1536973881.3199999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>176</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="24">
-        <v>72084432254.610001</v>
+        <v>5389815243.3499994</v>
       </c>
       <c r="D9" s="24">
-        <v>71866500770.459991</v>
+        <v>5373520318.0999994</v>
       </c>
       <c r="E9" s="24">
-        <v>71913722611.769989</v>
+        <v>5377051135.9499998</v>
       </c>
       <c r="F9" s="24">
-        <v>72992780327.459991</v>
+        <v>5457733213.0999994</v>
       </c>
       <c r="G9" s="24">
-        <v>73840398891</v>
+        <v>5521110385</v>
       </c>
       <c r="H9" s="24">
-        <v>74822817990.209991</v>
+        <v>5594566709.3499994</v>
       </c>
       <c r="I9" s="24">
-        <v>75735882075.869995</v>
+        <v>5662837299.4499998</v>
       </c>
       <c r="J9" s="24">
-        <v>76758974595.959991</v>
+        <v>5739334810.5999994</v>
       </c>
       <c r="K9" s="24">
-        <v>78049148455.889999</v>
+        <v>5835802224.1499996</v>
       </c>
       <c r="L9" s="24">
-        <v>79461451514.610001</v>
+        <v>5941401343.3499994</v>
       </c>
       <c r="M9" s="24">
-        <v>80932371156.659988</v>
+        <v>6051383275.0999994</v>
       </c>
       <c r="N9" s="24">
-        <v>82433011772.849991</v>
+        <v>6163587469.75</v>
       </c>
       <c r="O9" s="24">
-        <v>83897954334</v>
+        <v>6273122490</v>
       </c>
       <c r="P9" s="24">
-        <v>85439762491.349991</v>
+        <v>6388404817.25</v>
       </c>
       <c r="Q9" s="24">
-        <v>87106806486.75</v>
+        <v>6513051136.25</v>
       </c>
       <c r="R9" s="24">
-        <v>88924041591.719986</v>
+        <v>6648927374.1999998</v>
       </c>
       <c r="S9" s="24">
-        <v>90679934346.389999</v>
+        <v>6780216991.6499996</v>
       </c>
       <c r="T9" s="24">
-        <v>92331392035.229996</v>
+        <v>6903697909.0500002</v>
       </c>
       <c r="U9" s="24">
-        <v>94076499406.229996</v>
+        <v>7034181094.0500002</v>
       </c>
       <c r="V9" s="24">
-        <v>95730698989.979996</v>
+        <v>7157867025.3000002</v>
       </c>
       <c r="W9" s="24">
-        <v>97392235086.569992</v>
+        <v>7282101513.9499998</v>
       </c>
       <c r="X9" s="24">
-        <v>99195889056.419998</v>
+        <v>7416962278.6999998</v>
       </c>
       <c r="Y9" s="24">
-        <v>101082831833.7</v>
+        <v>7558050619.5</v>
       </c>
       <c r="Z9" s="24">
-        <v>102834947333.61</v>
+        <v>7689057808.3499994</v>
       </c>
       <c r="AA9" s="24">
-        <v>104728936134.24001</v>
+        <v>7830672986.3999996</v>
       </c>
       <c r="AB9" s="24">
-        <v>106615177304.67</v>
+        <v>7971708867.4499998</v>
       </c>
       <c r="AC9" s="24">
-        <v>108442061685.66</v>
+        <v>8108306590.0999994</v>
       </c>
       <c r="AD9" s="24">
-        <v>110186727196.71001</v>
+        <v>8238756736.8499994</v>
       </c>
       <c r="AE9" s="24">
-        <v>111955844551.23</v>
+        <v>8371035169.0499992</v>
       </c>
       <c r="AF9" s="24">
-        <v>113680129466.42999</v>
+        <v>8499961441.0499992</v>
       </c>
       <c r="AG9" s="24">
-        <v>115522381162.25999</v>
+        <v>8637708191.1000004</v>
       </c>
       <c r="AH9" s="24">
-        <v>117419705544.27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
+        <v>8779572773.4499989</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B11" s="16"/>
     </row>
   </sheetData>

</xml_diff>